<commit_message>
update manually check + get largest MW
</commit_message>
<xml_diff>
--- a/Reduction of ketone/manually check - 5,6cycloketone.xlsx
+++ b/Reduction of ketone/manually check - 5,6cycloketone.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suongsuong/Documents/GitHub/Reactivity-based-metric-of-complexity/Reduction of ketone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8C2526-8E03-844C-B600-CFD4963B591A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DA5229-3751-F94E-8FA6-17B8879C533B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34240" yWindow="-6940" windowWidth="29400" windowHeight="16220" xr2:uid="{BC994F64-CE92-9A46-9287-B4D99855AB55}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17100" xr2:uid="{BC994F64-CE92-9A46-9287-B4D99855AB55}"/>
   </bookViews>
   <sheets>
     <sheet name="full" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="65">
   <si>
     <t>wrong time</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>starting material is intermediate</t>
+  </si>
+  <si>
+    <t>meoh/water (check citation)</t>
   </si>
 </sst>
 </file>
@@ -642,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCB3314-64B3-6449-9FEB-FCB363FC8603}">
-  <dimension ref="A1:J133"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="106" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="106" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -968,11 +971,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="17">
-      <c r="A23">
-        <v>28195631</v>
+      <c r="A23" s="2">
+        <v>533786</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>7</v>
@@ -981,29 +984,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2">
-        <v>46605615</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0.71</v>
+    <row r="24" spans="1:4" ht="17">
+      <c r="A24">
+        <v>28195631</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>51891373</v>
+        <v>46605615</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="3">
-        <v>0.67</v>
+        <v>0.71</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -1011,33 +1014,35 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>4788828</v>
+        <v>51891373</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3">
-        <v>0.69</v>
+        <v>0.67</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17">
+    <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>4490693</v>
+        <v>4788828</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17">
       <c r="A28" s="2">
-        <v>4489690</v>
+        <v>4490693</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>63</v>
@@ -1048,81 +1053,79 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="17">
-      <c r="A29" s="5">
-        <v>49042116</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="3">
-        <v>0.52</v>
-      </c>
+      <c r="A29" s="2">
+        <v>4489690</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="3"/>
       <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="17">
       <c r="A30" s="5">
-        <v>38024254</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>34</v>
+        <v>49042116</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="C30" s="3">
-        <v>0.87</v>
-      </c>
-      <c r="D30" t="s">
-        <v>28</v>
+        <v>0.52</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="5">
+        <v>38024254</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="5">
         <v>3488969</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B32" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C32" s="3">
         <v>0.95</v>
-      </c>
-      <c r="D31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="21" customHeight="1">
-      <c r="A32" s="5">
-        <v>2623851</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="3">
-        <v>0.98</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:7" ht="21" customHeight="1">
       <c r="A33" s="5">
+        <v>2623851</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="D33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="5">
         <v>4900062</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="C33" s="7">
-        <v>2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="37" customHeight="1">
-      <c r="A34" s="5">
-        <v>4899619</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="C34" s="7">
         <v>2</v>
@@ -1131,209 +1134,214 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="47" customHeight="1">
+    <row r="35" spans="1:7" ht="38" customHeight="1">
       <c r="A35" s="5">
+        <v>4899619</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="47" customHeight="1">
+      <c r="A36" s="5">
         <v>3695571</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B36" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C36" s="3">
         <v>0.51</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="34">
-      <c r="A36" s="2">
+    <row r="37" spans="1:7" ht="34">
+      <c r="A37" s="2">
         <v>2164574</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B37" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C37" s="4">
         <v>0.31</v>
-      </c>
-      <c r="D36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="34">
-      <c r="A37" s="2">
-        <v>9092759</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="3">
-        <v>0.47</v>
       </c>
       <c r="D37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="34">
+      <c r="F37" s="2"/>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" ht="34">
       <c r="A38" s="2">
+        <v>9092759</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="34">
+      <c r="A39" s="2">
         <v>2227517</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B39" s="10" t="s">
         <v>10</v>
-      </c>
-      <c r="C38" s="7">
-        <v>3</v>
-      </c>
-      <c r="D38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="2">
-        <v>47458580</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="C39" s="7">
         <v>3</v>
       </c>
       <c r="D39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2">
+        <v>47458580</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="7">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="57" customHeight="1">
-      <c r="A40" s="5">
+    <row r="41" spans="1:7" ht="57" customHeight="1">
+      <c r="A41" s="5">
         <v>2549305</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B41" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="51">
-      <c r="A41" s="6">
-        <v>3601813</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>41</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16" customHeight="1">
+    <row r="42" spans="1:7" ht="51">
       <c r="A42" s="6">
-        <v>10426378</v>
+        <v>3601813</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="34">
-      <c r="A43" s="5">
-        <v>3195369</v>
+    <row r="43" spans="1:7" ht="16" customHeight="1">
+      <c r="A43" s="6">
+        <v>10426378</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44">
+    <row r="44" spans="1:7" ht="34">
+      <c r="A44" s="5">
+        <v>3195369</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
         <v>42647774</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B45" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45">
+    <row r="46" spans="1:7">
+      <c r="A46">
         <v>42647518</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B46" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>44</v>
       </c>
-      <c r="D45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="16" customHeight="1">
-      <c r="A46" s="5">
-        <v>9092667</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C46" s="6"/>
       <c r="D46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:7" ht="16" customHeight="1">
       <c r="A47" s="5">
+        <v>9092667</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="5">
         <v>9089729</v>
       </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="6" t="s">
+      <c r="B48" s="13"/>
+      <c r="C48" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="51">
-      <c r="A48" s="5">
+    <row r="49" spans="1:4" ht="51">
+      <c r="A49" s="5">
         <v>5171814</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B49" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="5">
-        <v>2568558</v>
-      </c>
-      <c r="B49" s="13"/>
       <c r="C49" s="6"/>
       <c r="D49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="5">
+        <v>2568558</v>
+      </c>
+      <c r="B50" s="13"/>
+      <c r="C50" s="6"/>
+      <c r="D50" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="2">
-        <v>35630033</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D50" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>47857344</v>
+        <v>35630033</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>48</v>
@@ -1344,7 +1352,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>54268031</v>
+        <v>47857344</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>48</v>
@@ -1355,10 +1363,10 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>8592817</v>
+        <v>54268031</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D53" t="s">
         <v>49</v>
@@ -1366,21 +1374,21 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>5103598</v>
+        <v>8592817</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D54" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>4645496</v>
+        <v>5103598</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D55" t="s">
         <v>59</v>
@@ -1388,10 +1396,10 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>9654587</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>52</v>
+        <v>4645496</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="D56" t="s">
         <v>59</v>
@@ -1399,10 +1407,10 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>36198566</v>
+        <v>9654587</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1410,23 +1418,26 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
+        <v>36198566</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="2">
         <v>9988006</v>
       </c>
-      <c r="D58" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59">
+      <c r="D59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
         <v>10252945</v>
-      </c>
-      <c r="D59" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="2">
-        <v>10252949</v>
       </c>
       <c r="D60" t="s">
         <v>58</v>
@@ -1434,7 +1445,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>41123517</v>
+        <v>10252949</v>
       </c>
       <c r="D61" t="s">
         <v>58</v>
@@ -1442,7 +1453,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>50751271</v>
+        <v>41123517</v>
       </c>
       <c r="D62" t="s">
         <v>58</v>
@@ -1450,7 +1461,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>50751266</v>
+        <v>50751271</v>
       </c>
       <c r="D63" t="s">
         <v>58</v>
@@ -1458,7 +1469,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>50751180</v>
+        <v>50751266</v>
       </c>
       <c r="D64" t="s">
         <v>58</v>
@@ -1466,7 +1477,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>8842757</v>
+        <v>50751180</v>
       </c>
       <c r="D65" t="s">
         <v>58</v>
@@ -1474,7 +1485,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>8645479</v>
+        <v>8842757</v>
       </c>
       <c r="D66" t="s">
         <v>58</v>
@@ -1482,7 +1493,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>9987915</v>
+        <v>8645479</v>
       </c>
       <c r="D67" t="s">
         <v>58</v>
@@ -1490,7 +1501,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>23063906</v>
+        <v>9987915</v>
       </c>
       <c r="D68" t="s">
         <v>58</v>
@@ -1498,7 +1509,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>29804781</v>
+        <v>23063906</v>
       </c>
       <c r="D69" t="s">
         <v>58</v>
@@ -1506,7 +1517,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>29804782</v>
+        <v>29804781</v>
       </c>
       <c r="D70" t="s">
         <v>58</v>
@@ -1514,7 +1525,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>144672</v>
+        <v>29804782</v>
       </c>
       <c r="D71" t="s">
         <v>58</v>
@@ -1522,7 +1533,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>58454081</v>
+        <v>144672</v>
       </c>
       <c r="D72" t="s">
         <v>58</v>
@@ -1530,7 +1541,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>9217498</v>
+        <v>58454081</v>
       </c>
       <c r="D73" t="s">
         <v>58</v>
@@ -1538,7 +1549,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>4587282</v>
+        <v>9217498</v>
       </c>
       <c r="D74" t="s">
         <v>58</v>
@@ -1546,7 +1557,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>28523993</v>
+        <v>4587282</v>
       </c>
       <c r="D75" t="s">
         <v>58</v>
@@ -1554,7 +1565,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>10347820</v>
+        <v>28523993</v>
       </c>
       <c r="D76" t="s">
         <v>58</v>
@@ -1562,7 +1573,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>10349806</v>
+        <v>10347820</v>
       </c>
       <c r="D77" t="s">
         <v>58</v>
@@ -1570,7 +1581,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>3931632</v>
+        <v>10349806</v>
       </c>
       <c r="D78" t="s">
         <v>58</v>
@@ -1578,7 +1589,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>3036530</v>
+        <v>3931632</v>
       </c>
       <c r="D79" t="s">
         <v>58</v>
@@ -1586,7 +1597,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>2823307</v>
+        <v>3036530</v>
       </c>
       <c r="D80" t="s">
         <v>58</v>
@@ -1594,7 +1605,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>27930070</v>
+        <v>2823307</v>
       </c>
       <c r="D81" t="s">
         <v>58</v>
@@ -1602,7 +1613,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>27978138</v>
+        <v>27930070</v>
       </c>
       <c r="D82" t="s">
         <v>58</v>
@@ -1610,7 +1621,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>27978134</v>
+        <v>27978138</v>
       </c>
       <c r="D83" t="s">
         <v>58</v>
@@ -1618,7 +1629,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>50167721</v>
+        <v>27978134</v>
       </c>
       <c r="D84" t="s">
         <v>58</v>
@@ -1626,7 +1637,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>11236288</v>
+        <v>50167721</v>
       </c>
       <c r="D85" t="s">
         <v>58</v>
@@ -1634,7 +1645,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>33412557</v>
+        <v>11236288</v>
       </c>
       <c r="D86" t="s">
         <v>58</v>
@@ -1642,7 +1653,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>38188034</v>
+        <v>33412557</v>
       </c>
       <c r="D87" t="s">
         <v>58</v>
@@ -1650,7 +1661,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>46723145</v>
+        <v>38188034</v>
       </c>
       <c r="D88" t="s">
         <v>58</v>
@@ -1658,7 +1669,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>35043483</v>
+        <v>46723145</v>
       </c>
       <c r="D89" t="s">
         <v>58</v>
@@ -1666,7 +1677,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>8847498</v>
+        <v>35043483</v>
       </c>
       <c r="D90" t="s">
         <v>58</v>
@@ -1674,7 +1685,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>9847882</v>
+        <v>8847498</v>
       </c>
       <c r="D91" t="s">
         <v>58</v>
@@ -1682,7 +1693,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>55768198</v>
+        <v>9847882</v>
       </c>
       <c r="D92" t="s">
         <v>58</v>
@@ -1690,7 +1701,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>9624111</v>
+        <v>55768198</v>
       </c>
       <c r="D93" t="s">
         <v>58</v>
@@ -1698,7 +1709,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>4872121</v>
+        <v>9624111</v>
       </c>
       <c r="D94" t="s">
         <v>58</v>
@@ -1706,7 +1717,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>855271</v>
+        <v>4872121</v>
       </c>
       <c r="D95" t="s">
         <v>58</v>
@@ -1714,7 +1725,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>3122232</v>
+        <v>855271</v>
       </c>
       <c r="D96" t="s">
         <v>58</v>
@@ -1722,7 +1733,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>4289070</v>
+        <v>3122232</v>
       </c>
       <c r="D97" t="s">
         <v>58</v>
@@ -1730,7 +1741,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>4898806</v>
+        <v>4289070</v>
       </c>
       <c r="D98" t="s">
         <v>58</v>
@@ -1738,7 +1749,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>4277588</v>
+        <v>4898806</v>
       </c>
       <c r="D99" t="s">
         <v>58</v>
@@ -1746,7 +1757,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>4743278</v>
+        <v>4277588</v>
       </c>
       <c r="D100" t="s">
         <v>58</v>
@@ -1754,7 +1765,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>39856777</v>
+        <v>4743278</v>
       </c>
       <c r="D101" t="s">
         <v>58</v>
@@ -1762,7 +1773,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>5345001</v>
+        <v>39856777</v>
       </c>
       <c r="D102" t="s">
         <v>58</v>
@@ -1770,7 +1781,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>2839566</v>
+        <v>5345001</v>
       </c>
       <c r="D103" t="s">
         <v>58</v>
@@ -1778,7 +1789,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>3108523</v>
+        <v>2839566</v>
       </c>
       <c r="D104" t="s">
         <v>58</v>
@@ -1786,7 +1797,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>10510153</v>
+        <v>3108523</v>
       </c>
       <c r="D105" t="s">
         <v>58</v>
@@ -1794,7 +1805,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>50124439</v>
+        <v>10510153</v>
       </c>
       <c r="D106" t="s">
         <v>58</v>
@@ -1802,7 +1813,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>29252231</v>
+        <v>50124439</v>
       </c>
       <c r="D107" t="s">
         <v>58</v>
@@ -1810,7 +1821,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>28530018</v>
+        <v>29252231</v>
       </c>
       <c r="D108" t="s">
         <v>58</v>
@@ -1818,7 +1829,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>4444115</v>
+        <v>28530018</v>
       </c>
       <c r="D109" t="s">
         <v>58</v>
@@ -1826,7 +1837,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>42996751</v>
+        <v>4444115</v>
       </c>
       <c r="D110" t="s">
         <v>58</v>
@@ -1834,7 +1845,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>4594355</v>
+        <v>42996751</v>
       </c>
       <c r="D111" t="s">
         <v>58</v>
@@ -1842,7 +1853,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>2125516</v>
+        <v>4594355</v>
       </c>
       <c r="D112" t="s">
         <v>58</v>
@@ -1850,7 +1861,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>42093911</v>
+        <v>2125516</v>
       </c>
       <c r="D113" t="s">
         <v>58</v>
@@ -1858,7 +1869,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>2206858</v>
+        <v>42093911</v>
       </c>
       <c r="D114" t="s">
         <v>58</v>
@@ -1866,7 +1877,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>731611</v>
+        <v>2206858</v>
       </c>
       <c r="D115" t="s">
         <v>58</v>
@@ -1874,7 +1885,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>2125887</v>
+        <v>731611</v>
       </c>
       <c r="D116" t="s">
         <v>58</v>
@@ -1882,7 +1893,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>4993066</v>
+        <v>2125887</v>
       </c>
       <c r="D117" t="s">
         <v>58</v>
@@ -1890,7 +1901,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>2207264</v>
+        <v>4993066</v>
       </c>
       <c r="D118" t="s">
         <v>58</v>
@@ -1898,7 +1909,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>5015112</v>
+        <v>2207264</v>
       </c>
       <c r="D119" t="s">
         <v>58</v>
@@ -1906,7 +1917,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>9750769</v>
+        <v>5015112</v>
       </c>
       <c r="D120" t="s">
         <v>58</v>
@@ -1914,7 +1925,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>8785468</v>
+        <v>9750769</v>
       </c>
       <c r="D121" t="s">
         <v>58</v>
@@ -1922,7 +1933,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>3572764</v>
+        <v>8785468</v>
       </c>
       <c r="D122" t="s">
         <v>58</v>
@@ -1930,7 +1941,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>25948486</v>
+        <v>3572764</v>
       </c>
       <c r="D123" t="s">
         <v>58</v>
@@ -1938,7 +1949,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>9653123</v>
+        <v>25948486</v>
       </c>
       <c r="D124" t="s">
         <v>58</v>
@@ -1946,7 +1957,7 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>9496014</v>
+        <v>9653123</v>
       </c>
       <c r="D125" t="s">
         <v>58</v>
@@ -1954,7 +1965,7 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>49973963</v>
+        <v>9496014</v>
       </c>
       <c r="D126" t="s">
         <v>58</v>
@@ -1962,7 +1973,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>5174026</v>
+        <v>49973963</v>
       </c>
       <c r="D127" t="s">
         <v>58</v>
@@ -1970,7 +1981,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>5223356</v>
+        <v>5174026</v>
       </c>
       <c r="D128" t="s">
         <v>58</v>
@@ -1978,7 +1989,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>10263413</v>
+        <v>5223356</v>
       </c>
       <c r="D129" t="s">
         <v>58</v>
@@ -1986,7 +1997,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>3235197</v>
+        <v>10263413</v>
       </c>
       <c r="D130" t="s">
         <v>58</v>
@@ -1994,7 +2005,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>32544299</v>
+        <v>3235197</v>
       </c>
       <c r="D131" t="s">
         <v>58</v>
@@ -2002,7 +2013,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>3636182</v>
+        <v>32544299</v>
       </c>
       <c r="D132" t="s">
         <v>58</v>
@@ -2010,9 +2021,17 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
+        <v>3636182</v>
+      </c>
+      <c r="D133" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="2">
         <v>5151201</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D134" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>